<commit_message>
Added log, fixed bug, started scrapping'
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="HP_Test" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HP" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,6 +555,31 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ACM029T0XJ</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>HPE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>MSA 1050</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Q2R21B</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>